<commit_message>
Rounding quantities for aggregate transactions
</commit_message>
<xml_diff>
--- a/Data/Sterling -- transactions.xlsx
+++ b/Data/Sterling -- transactions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Portfolio-management\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Y\Portfolio management\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{334CF986-2555-497B-808C-32ADEE5B3DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E902B34-AFE3-4E39-9EA7-58D8C7843C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" xr2:uid="{89906832-8650-41E7-B054-7F68D86C6C3B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{89906832-8650-41E7-B054-7F68D86C6C3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Транзакции_Sterling" sheetId="1" r:id="rId1"/>
@@ -199,12 +199,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="yyyy"/>
     <numFmt numFmtId="165" formatCode="#,##0.0_);\(#,##0.0\)"/>
     <numFmt numFmtId="166" formatCode="0.0%"/>
     <numFmt numFmtId="167" formatCode="#,##0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.000"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -346,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -564,14 +563,6 @@
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="37" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,7 +581,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Портфель"/>
@@ -1332,136 +1323,136 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99646042-A90C-400A-8964-D5FAE7C7EB72}">
   <sheetPr codeName="Sheet148"/>
-  <dimension ref="A1:DW63"/>
+  <dimension ref="A1:DW56"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N48" sqref="N48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" outlineLevelRow="1" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="11.64453125" customWidth="1"/>
-    <col min="5" max="5" width="2.76171875" customWidth="1"/>
-    <col min="6" max="6" width="2.76171875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.64453125" customWidth="1"/>
-    <col min="8" max="8" width="9.41015625" customWidth="1"/>
-    <col min="9" max="9" width="8.3515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.29296875" style="2" customWidth="1"/>
+    <col min="1" max="4" width="11.7109375" customWidth="1"/>
+    <col min="5" max="5" width="2.7109375" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.7109375" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" customWidth="1"/>
+    <col min="9" max="9" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.28515625" style="2" customWidth="1"/>
     <col min="12" max="12" width="7" customWidth="1"/>
-    <col min="13" max="13" width="12.8203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="9.76171875" customWidth="1"/>
-    <col min="16" max="16" width="11.1171875" customWidth="1"/>
-    <col min="17" max="17" width="1.703125" customWidth="1"/>
-    <col min="18" max="18" width="11.64453125" customWidth="1"/>
-    <col min="19" max="19" width="9.41015625" customWidth="1"/>
-    <col min="20" max="20" width="8.3515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.29296875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="9.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.140625" customWidth="1"/>
+    <col min="17" max="17" width="1.7109375" customWidth="1"/>
+    <col min="18" max="18" width="11.7109375" customWidth="1"/>
+    <col min="19" max="19" width="9.42578125" customWidth="1"/>
+    <col min="20" max="20" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.28515625" style="2" customWidth="1"/>
     <col min="23" max="23" width="7" customWidth="1"/>
-    <col min="24" max="24" width="12.8203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="26" width="9.76171875" customWidth="1"/>
-    <col min="27" max="27" width="11.1171875" customWidth="1"/>
-    <col min="28" max="28" width="1.703125" customWidth="1"/>
-    <col min="29" max="29" width="11.64453125" customWidth="1"/>
-    <col min="30" max="30" width="9.41015625" customWidth="1"/>
-    <col min="31" max="31" width="8.3515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.29296875" style="2" customWidth="1"/>
+    <col min="24" max="24" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="26" width="9.7109375" customWidth="1"/>
+    <col min="27" max="27" width="11.140625" customWidth="1"/>
+    <col min="28" max="28" width="1.7109375" customWidth="1"/>
+    <col min="29" max="29" width="11.7109375" customWidth="1"/>
+    <col min="30" max="30" width="9.42578125" customWidth="1"/>
+    <col min="31" max="31" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.28515625" style="2" customWidth="1"/>
     <col min="34" max="34" width="7" customWidth="1"/>
-    <col min="35" max="35" width="12.8203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="37" width="9.76171875" customWidth="1"/>
-    <col min="38" max="38" width="11.1171875" customWidth="1"/>
-    <col min="39" max="39" width="1.703125" customWidth="1"/>
-    <col min="40" max="40" width="11.64453125" customWidth="1"/>
-    <col min="41" max="41" width="9.41015625" customWidth="1"/>
-    <col min="42" max="42" width="8.3515625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="7.29296875" style="2" customWidth="1"/>
+    <col min="35" max="35" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="9.7109375" customWidth="1"/>
+    <col min="38" max="38" width="11.140625" customWidth="1"/>
+    <col min="39" max="39" width="1.7109375" customWidth="1"/>
+    <col min="40" max="40" width="11.7109375" customWidth="1"/>
+    <col min="41" max="41" width="9.42578125" customWidth="1"/>
+    <col min="42" max="42" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="7.28515625" style="2" customWidth="1"/>
     <col min="45" max="45" width="7" customWidth="1"/>
-    <col min="46" max="46" width="12.8203125" bestFit="1" customWidth="1"/>
-    <col min="47" max="48" width="9.76171875" customWidth="1"/>
-    <col min="49" max="49" width="11.1171875" customWidth="1"/>
-    <col min="50" max="50" width="1.703125" customWidth="1"/>
-    <col min="51" max="51" width="11.64453125" customWidth="1"/>
-    <col min="52" max="52" width="9.41015625" customWidth="1"/>
-    <col min="53" max="53" width="8.3515625" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="7.29296875" style="2" customWidth="1"/>
+    <col min="46" max="46" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="47" max="48" width="9.7109375" customWidth="1"/>
+    <col min="49" max="49" width="11.140625" customWidth="1"/>
+    <col min="50" max="50" width="1.7109375" customWidth="1"/>
+    <col min="51" max="51" width="11.7109375" customWidth="1"/>
+    <col min="52" max="52" width="9.42578125" customWidth="1"/>
+    <col min="53" max="53" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="7.28515625" style="2" customWidth="1"/>
     <col min="56" max="56" width="7" customWidth="1"/>
-    <col min="57" max="57" width="12.8203125" bestFit="1" customWidth="1"/>
-    <col min="58" max="59" width="9.76171875" customWidth="1"/>
-    <col min="60" max="60" width="11.1171875" customWidth="1"/>
-    <col min="61" max="61" width="1.703125" customWidth="1"/>
-    <col min="62" max="62" width="11.64453125" customWidth="1"/>
-    <col min="63" max="63" width="9.41015625" customWidth="1"/>
-    <col min="64" max="64" width="8.3515625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="7.29296875" style="2" customWidth="1"/>
+    <col min="57" max="57" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="59" width="9.7109375" customWidth="1"/>
+    <col min="60" max="60" width="11.140625" customWidth="1"/>
+    <col min="61" max="61" width="1.7109375" customWidth="1"/>
+    <col min="62" max="62" width="11.7109375" customWidth="1"/>
+    <col min="63" max="63" width="9.42578125" customWidth="1"/>
+    <col min="64" max="64" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="7.28515625" style="2" customWidth="1"/>
     <col min="67" max="67" width="7" customWidth="1"/>
-    <col min="68" max="68" width="12.8203125" bestFit="1" customWidth="1"/>
-    <col min="69" max="70" width="9.76171875" customWidth="1"/>
-    <col min="71" max="71" width="11.1171875" customWidth="1"/>
-    <col min="72" max="72" width="1.703125" customWidth="1"/>
-    <col min="73" max="73" width="11.64453125" customWidth="1"/>
-    <col min="74" max="74" width="9.41015625" customWidth="1"/>
-    <col min="75" max="75" width="8.3515625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="7.29296875" style="2" customWidth="1"/>
+    <col min="68" max="68" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="69" max="70" width="9.7109375" customWidth="1"/>
+    <col min="71" max="71" width="11.140625" customWidth="1"/>
+    <col min="72" max="72" width="1.7109375" customWidth="1"/>
+    <col min="73" max="73" width="11.7109375" customWidth="1"/>
+    <col min="74" max="74" width="9.42578125" customWidth="1"/>
+    <col min="75" max="75" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="7.28515625" style="2" customWidth="1"/>
     <col min="78" max="78" width="7" customWidth="1"/>
-    <col min="79" max="79" width="12.8203125" bestFit="1" customWidth="1"/>
-    <col min="80" max="81" width="9.76171875" customWidth="1"/>
-    <col min="82" max="82" width="11.1171875" customWidth="1"/>
-    <col min="83" max="83" width="1.703125" customWidth="1"/>
-    <col min="84" max="84" width="11.64453125" customWidth="1"/>
-    <col min="85" max="85" width="9.41015625" customWidth="1"/>
-    <col min="86" max="86" width="8.3515625" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="7.29296875" style="2" customWidth="1"/>
+    <col min="79" max="79" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="81" width="9.7109375" customWidth="1"/>
+    <col min="82" max="82" width="11.140625" customWidth="1"/>
+    <col min="83" max="83" width="1.7109375" customWidth="1"/>
+    <col min="84" max="84" width="11.7109375" customWidth="1"/>
+    <col min="85" max="85" width="9.42578125" customWidth="1"/>
+    <col min="86" max="86" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="7.28515625" style="2" customWidth="1"/>
     <col min="89" max="89" width="7" customWidth="1"/>
-    <col min="90" max="90" width="12.8203125" bestFit="1" customWidth="1"/>
-    <col min="91" max="92" width="9.76171875" customWidth="1"/>
-    <col min="93" max="93" width="11.1171875" customWidth="1"/>
-    <col min="94" max="94" width="1.703125" customWidth="1"/>
-    <col min="95" max="95" width="11.64453125" customWidth="1"/>
-    <col min="96" max="96" width="9.41015625" customWidth="1"/>
-    <col min="97" max="97" width="8.3515625" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="7.29296875" style="2" customWidth="1"/>
+    <col min="90" max="90" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="91" max="92" width="9.7109375" customWidth="1"/>
+    <col min="93" max="93" width="11.140625" customWidth="1"/>
+    <col min="94" max="94" width="1.7109375" customWidth="1"/>
+    <col min="95" max="95" width="11.7109375" customWidth="1"/>
+    <col min="96" max="96" width="9.42578125" customWidth="1"/>
+    <col min="97" max="97" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="99" max="99" width="7.28515625" style="2" customWidth="1"/>
     <col min="100" max="100" width="7" customWidth="1"/>
-    <col min="101" max="101" width="12.8203125" bestFit="1" customWidth="1"/>
-    <col min="102" max="103" width="9.76171875" customWidth="1"/>
-    <col min="104" max="104" width="11.1171875" customWidth="1"/>
-    <col min="105" max="105" width="1.703125" customWidth="1"/>
-    <col min="106" max="106" width="11.64453125" customWidth="1"/>
-    <col min="107" max="107" width="9.41015625" customWidth="1"/>
-    <col min="108" max="108" width="8.3515625" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="7.29296875" style="2" customWidth="1"/>
+    <col min="101" max="101" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="102" max="103" width="9.7109375" customWidth="1"/>
+    <col min="104" max="104" width="11.140625" customWidth="1"/>
+    <col min="105" max="105" width="1.7109375" customWidth="1"/>
+    <col min="106" max="106" width="11.7109375" customWidth="1"/>
+    <col min="107" max="107" width="9.42578125" customWidth="1"/>
+    <col min="108" max="108" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="110" max="110" width="7.28515625" style="2" customWidth="1"/>
     <col min="111" max="111" width="7" customWidth="1"/>
-    <col min="112" max="112" width="12.8203125" bestFit="1" customWidth="1"/>
-    <col min="113" max="114" width="9.76171875" customWidth="1"/>
-    <col min="115" max="115" width="11.1171875" customWidth="1"/>
-    <col min="116" max="116" width="1.703125" customWidth="1"/>
-    <col min="117" max="117" width="11.64453125" customWidth="1"/>
-    <col min="118" max="118" width="9.41015625" customWidth="1"/>
-    <col min="119" max="119" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="9.64453125" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="7.29296875" style="2" customWidth="1"/>
+    <col min="112" max="112" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="113" max="114" width="9.7109375" customWidth="1"/>
+    <col min="115" max="115" width="11.140625" customWidth="1"/>
+    <col min="116" max="116" width="1.7109375" customWidth="1"/>
+    <col min="117" max="117" width="11.7109375" customWidth="1"/>
+    <col min="118" max="118" width="9.42578125" customWidth="1"/>
+    <col min="119" max="119" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="121" max="121" width="7.28515625" style="2" customWidth="1"/>
     <col min="122" max="122" width="7" customWidth="1"/>
-    <col min="123" max="123" width="12.8203125" bestFit="1" customWidth="1"/>
-    <col min="124" max="125" width="9.76171875" customWidth="1"/>
-    <col min="126" max="126" width="11.1171875" customWidth="1"/>
-    <col min="127" max="127" width="1.703125" customWidth="1"/>
+    <col min="123" max="123" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="124" max="125" width="9.7109375" customWidth="1"/>
+    <col min="126" max="126" width="11.140625" customWidth="1"/>
+    <col min="127" max="127" width="1.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:127" x14ac:dyDescent="0.25">
       <c r="F1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="DJ1" s="3"/>
     </row>
-    <row r="2" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1611,7 +1602,7 @@
       <c r="DV2" s="4"/>
       <c r="DW2" s="4"/>
     </row>
-    <row r="3" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1761,7 +1752,7 @@
       <c r="DV3" s="6"/>
       <c r="DW3" s="4"/>
     </row>
-    <row r="4" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A4" s="9"/>
       <c r="B4" s="10"/>
       <c r="C4" s="10"/>
@@ -1988,7 +1979,7 @@
       </c>
       <c r="DW4" s="11"/>
     </row>
-    <row r="5" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -2204,7 +2195,7 @@
       </c>
       <c r="DW5" s="11"/>
     </row>
-    <row r="6" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>41274</v>
       </c>
@@ -2356,7 +2347,7 @@
       <c r="DV6" s="18"/>
       <c r="DW6" s="19"/>
     </row>
-    <row r="7" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A7" s="9"/>
       <c r="B7" s="9"/>
       <c r="C7" s="9"/>
@@ -2561,7 +2552,7 @@
       </c>
       <c r="DW7" s="23"/>
     </row>
-    <row r="8" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="24"/>
       <c r="C8" s="24"/>
@@ -2788,7 +2779,7 @@
       </c>
       <c r="DW8" s="23"/>
     </row>
-    <row r="9" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>29</v>
       </c>
@@ -3034,7 +3025,7 @@
       </c>
       <c r="DW9" s="11"/>
     </row>
-    <row r="10" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>30</v>
       </c>
@@ -3214,7 +3205,7 @@
       <c r="DV10" s="11"/>
       <c r="DW10" s="11"/>
     </row>
-    <row r="11" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>32</v>
       </c>
@@ -3394,7 +3385,7 @@
       <c r="DV11" s="11"/>
       <c r="DW11" s="11"/>
     </row>
-    <row r="12" spans="1:127" s="34" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:127" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
       <c r="E12" s="9"/>
@@ -3609,7 +3600,7 @@
       </c>
       <c r="DW12" s="11"/>
     </row>
-    <row r="13" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A13" s="9"/>
       <c r="B13" s="26"/>
       <c r="C13" s="39"/>
@@ -3826,7 +3817,7 @@
       </c>
       <c r="DW13" s="43"/>
     </row>
-    <row r="14" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A14" s="9"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -4031,7 +4022,7 @@
       </c>
       <c r="DW14" s="45"/>
     </row>
-    <row r="15" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>36</v>
       </c>
@@ -4183,7 +4174,7 @@
       <c r="DV15" s="18"/>
       <c r="DW15" s="19"/>
     </row>
-    <row r="16" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -4388,7 +4379,7 @@
       </c>
       <c r="DW16" s="11"/>
     </row>
-    <row r="17" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="17" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -4615,7 +4606,7 @@
       </c>
       <c r="DW17" s="11"/>
     </row>
-    <row r="18" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>29</v>
       </c>
@@ -4861,7 +4852,7 @@
       </c>
       <c r="DW18" s="11"/>
     </row>
-    <row r="19" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>30</v>
       </c>
@@ -5085,7 +5076,7 @@
       </c>
       <c r="DW19" s="11"/>
     </row>
-    <row r="20" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
         <v>32</v>
       </c>
@@ -5309,7 +5300,7 @@
       </c>
       <c r="DW20" s="11"/>
     </row>
-    <row r="21" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -5525,7 +5516,7 @@
       </c>
       <c r="DW21" s="11"/>
     </row>
-    <row r="22" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="22" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A22" s="39"/>
       <c r="B22" s="39"/>
       <c r="C22" s="39"/>
@@ -5742,7 +5733,7 @@
       </c>
       <c r="DW22" s="43"/>
     </row>
-    <row r="23" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -5947,7 +5938,7 @@
       </c>
       <c r="DW23" s="45"/>
     </row>
-    <row r="24" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -6031,7 +6022,7 @@
       <c r="DR24" s="4"/>
       <c r="DS24" s="4"/>
     </row>
-    <row r="25" spans="1:127" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A25" s="49"/>
       <c r="B25" s="49"/>
       <c r="C25" s="49"/>
@@ -6357,7 +6348,7 @@
       </c>
       <c r="DW25" s="49"/>
     </row>
-    <row r="26" spans="1:127" s="60" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:127" s="60" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="53"/>
       <c r="B26" s="54"/>
       <c r="C26" s="53"/>
@@ -6371,7 +6362,7 @@
         <v>24.5</v>
       </c>
       <c r="I26" s="56">
-        <v>4.0829085619868453</v>
+        <v>4.0829079999999998</v>
       </c>
       <c r="J26" s="57"/>
       <c r="K26" s="58"/>
@@ -6640,7 +6631,7 @@
       </c>
       <c r="DW26" s="58"/>
     </row>
-    <row r="27" spans="1:127" s="60" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="27" spans="1:127" s="60" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="53"/>
       <c r="B27" s="53"/>
       <c r="C27" s="53"/>
@@ -6923,7 +6914,7 @@
       </c>
       <c r="DW27" s="58"/>
     </row>
-    <row r="28" spans="1:127" s="60" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:127" s="60" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="53"/>
       <c r="B28" s="53"/>
       <c r="C28" s="53"/>
@@ -7206,7 +7197,7 @@
       </c>
       <c r="DW28" s="58"/>
     </row>
-    <row r="29" spans="1:127" s="60" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:127" s="60" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A29" s="53"/>
       <c r="B29" s="53"/>
       <c r="C29" s="53"/>
@@ -7489,7 +7480,7 @@
       </c>
       <c r="DW29" s="58"/>
     </row>
-    <row r="30" spans="1:127" s="60" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:127" s="60" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="53"/>
       <c r="B30" s="53"/>
       <c r="C30" s="53"/>
@@ -7772,7 +7763,7 @@
       </c>
       <c r="DW30" s="58"/>
     </row>
-    <row r="31" spans="1:127" s="60" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:127" s="60" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A31" s="53"/>
       <c r="B31" s="53"/>
       <c r="C31" s="53"/>
@@ -8055,7 +8046,7 @@
       </c>
       <c r="DW31" s="58"/>
     </row>
-    <row r="32" spans="1:127" s="60" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="32" spans="1:127" s="60" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="53"/>
       <c r="B32" s="53"/>
       <c r="C32" s="53"/>
@@ -8338,7 +8329,7 @@
       </c>
       <c r="DW32" s="58"/>
     </row>
-    <row r="33" spans="1:127" s="60" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:127" s="60" customFormat="1" outlineLevel="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A33" s="53"/>
       <c r="B33" s="53"/>
       <c r="C33" s="53"/>
@@ -8621,7 +8612,7 @@
       </c>
       <c r="DW33" s="58"/>
     </row>
-    <row r="34" spans="1:127" s="60" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:127" s="60" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="53"/>
       <c r="B34" s="53"/>
       <c r="C34" s="53"/>
@@ -8904,7 +8895,7 @@
       </c>
       <c r="DW34" s="58"/>
     </row>
-    <row r="35" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="53"/>
       <c r="B35" s="53"/>
       <c r="C35" s="53"/>
@@ -9187,7 +9178,7 @@
       </c>
       <c r="DW35" s="58"/>
     </row>
-    <row r="36" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="53"/>
       <c r="B36" s="53"/>
       <c r="C36" s="53"/>
@@ -9470,7 +9461,7 @@
       </c>
       <c r="DW36" s="58"/>
     </row>
-    <row r="37" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="53"/>
       <c r="B37" s="53"/>
       <c r="C37" s="53"/>
@@ -9753,7 +9744,7 @@
       </c>
       <c r="DW37" s="58"/>
     </row>
-    <row r="38" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="53"/>
       <c r="B38" s="53"/>
       <c r="C38" s="53"/>
@@ -10036,7 +10027,7 @@
       </c>
       <c r="DW38" s="58"/>
     </row>
-    <row r="39" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="53"/>
       <c r="B39" s="53"/>
       <c r="C39" s="53"/>
@@ -10319,7 +10310,7 @@
       </c>
       <c r="DW39" s="58"/>
     </row>
-    <row r="40" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="53"/>
       <c r="B40" s="53"/>
       <c r="C40" s="53"/>
@@ -10602,7 +10593,7 @@
       </c>
       <c r="DW40" s="58"/>
     </row>
-    <row r="41" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="53"/>
       <c r="B41" s="53"/>
       <c r="C41" s="53"/>
@@ -10885,7 +10876,7 @@
       </c>
       <c r="DW41" s="58"/>
     </row>
-    <row r="42" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="42" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="53"/>
       <c r="B42" s="53"/>
       <c r="C42" s="53"/>
@@ -11168,7 +11159,7 @@
       </c>
       <c r="DW42" s="58"/>
     </row>
-    <row r="43" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="53"/>
       <c r="B43" s="53"/>
       <c r="C43" s="53"/>
@@ -11451,7 +11442,7 @@
       </c>
       <c r="DW43" s="58"/>
     </row>
-    <row r="44" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="53"/>
       <c r="B44" s="53"/>
       <c r="C44" s="53"/>
@@ -11734,7 +11725,7 @@
       </c>
       <c r="DW44" s="58"/>
     </row>
-    <row r="45" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="53"/>
       <c r="B45" s="53"/>
       <c r="C45" s="53"/>
@@ -12017,7 +12008,7 @@
       </c>
       <c r="DW45" s="58"/>
     </row>
-    <row r="46" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="53"/>
       <c r="B46" s="53"/>
       <c r="C46" s="53"/>
@@ -12300,7 +12291,7 @@
       </c>
       <c r="DW46" s="58"/>
     </row>
-    <row r="47" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="47" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="53"/>
       <c r="B47" s="53"/>
       <c r="C47" s="53"/>
@@ -12583,7 +12574,7 @@
       </c>
       <c r="DW47" s="58"/>
     </row>
-    <row r="48" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="53"/>
       <c r="B48" s="53"/>
       <c r="C48" s="53"/>
@@ -12866,7 +12857,7 @@
       </c>
       <c r="DW48" s="58"/>
     </row>
-    <row r="49" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="53"/>
       <c r="B49" s="53"/>
       <c r="C49" s="53"/>
@@ -13149,7 +13140,7 @@
       </c>
       <c r="DW49" s="58"/>
     </row>
-    <row r="50" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="53"/>
       <c r="B50" s="53"/>
       <c r="C50" s="53"/>
@@ -13245,7 +13236,7 @@
       <c r="DV50" s="58"/>
       <c r="DW50" s="58"/>
     </row>
-    <row r="51" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
@@ -13259,7 +13250,7 @@
         <v>24.65</v>
       </c>
       <c r="I51" s="57">
-        <v>15.511726349730367</v>
+        <v>-15.511726349730401</v>
       </c>
       <c r="J51" s="58"/>
       <c r="K51" s="58"/>
@@ -13283,7 +13274,7 @@
         <v>2.2400000000000002</v>
       </c>
       <c r="T51" s="58">
-        <v>535.41392108885907</v>
+        <v>-535.41392108885896</v>
       </c>
       <c r="U51" s="58"/>
       <c r="V51" s="58"/>
@@ -13307,7 +13298,7 @@
         <v>1.32</v>
       </c>
       <c r="AE51" s="58">
-        <v>328.41514840550707</v>
+        <v>-328.41514840550701</v>
       </c>
       <c r="AF51" s="58"/>
       <c r="AG51" s="58"/>
@@ -13331,7 +13322,7 @@
         <v>4.0999999999999996</v>
       </c>
       <c r="AP51" s="58">
-        <v>170.83142267799983</v>
+        <v>-170.831422678</v>
       </c>
       <c r="AQ51" s="58"/>
       <c r="AR51" s="58"/>
@@ -13355,7 +13346,7 @@
         <v>369.16</v>
       </c>
       <c r="BA51" s="58">
-        <v>3.6228925052792933</v>
+        <v>-3.6228925052792902</v>
       </c>
       <c r="BB51" s="58"/>
       <c r="BC51" s="58"/>
@@ -13379,7 +13370,7 @@
         <v>2.5</v>
       </c>
       <c r="BL51" s="58">
-        <v>361.53880374303179</v>
+        <v>-361.53880374303202</v>
       </c>
       <c r="BM51" s="58"/>
       <c r="BN51" s="58"/>
@@ -13403,7 +13394,7 @@
         <v>1.58</v>
       </c>
       <c r="BW51" s="58">
-        <v>523.57460574615516</v>
+        <v>-523.57460574615504</v>
       </c>
       <c r="BX51" s="58"/>
       <c r="BY51" s="58"/>
@@ -13427,7 +13418,7 @@
         <v>253.74</v>
       </c>
       <c r="CH51" s="58">
-        <v>1.6153468295855311</v>
+        <v>-1.61534682958553</v>
       </c>
       <c r="CI51" s="58"/>
       <c r="CJ51" s="58"/>
@@ -13451,7 +13442,7 @@
         <v>6.97</v>
       </c>
       <c r="CS51" s="58">
-        <v>41.965713867296444</v>
+        <v>-41.965713867296401</v>
       </c>
       <c r="CT51" s="58"/>
       <c r="CU51" s="58"/>
@@ -13475,7 +13466,7 @@
         <v>215.75</v>
       </c>
       <c r="DD51" s="58">
-        <v>1.6194754309215404</v>
+        <v>-1.61947543092154</v>
       </c>
       <c r="DE51" s="58"/>
       <c r="DF51" s="58"/>
@@ -13499,7 +13490,7 @@
         <v>519.79999999999995</v>
       </c>
       <c r="DO51" s="55">
-        <v>2.4664308626762574</v>
+        <v>-2.4664308626762601</v>
       </c>
       <c r="DP51" s="58"/>
       <c r="DQ51" s="58"/>
@@ -13517,15 +13508,15 @@
       </c>
       <c r="DW51" s="58"/>
     </row>
-    <row r="52" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="52" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="79"/>
       <c r="B52" s="79"/>
       <c r="C52" s="79"/>
       <c r="D52" s="80"/>
       <c r="E52"/>
       <c r="F52" s="1"/>
-      <c r="G52" s="81"/>
-      <c r="H52" s="82"/>
+      <c r="G52" s="53"/>
+      <c r="H52"/>
       <c r="I52"/>
       <c r="J52"/>
       <c r="K52" s="2"/>
@@ -13533,10 +13524,10 @@
       <c r="M52" s="2"/>
       <c r="N52"/>
       <c r="O52"/>
-      <c r="P52"/>
-      <c r="Q52"/>
-      <c r="R52" s="81"/>
-      <c r="S52" s="82"/>
+      <c r="P52" s="2"/>
+      <c r="Q52" s="2"/>
+      <c r="R52" s="53"/>
+      <c r="S52"/>
       <c r="T52"/>
       <c r="U52"/>
       <c r="V52" s="2"/>
@@ -13544,10 +13535,10 @@
       <c r="X52" s="2"/>
       <c r="Y52"/>
       <c r="Z52"/>
-      <c r="AA52"/>
-      <c r="AB52"/>
-      <c r="AC52" s="81"/>
-      <c r="AD52" s="82"/>
+      <c r="AA52" s="2"/>
+      <c r="AB52" s="2"/>
+      <c r="AC52" s="53"/>
+      <c r="AD52"/>
       <c r="AE52"/>
       <c r="AF52"/>
       <c r="AG52" s="2"/>
@@ -13555,10 +13546,10 @@
       <c r="AI52" s="2"/>
       <c r="AJ52"/>
       <c r="AK52"/>
-      <c r="AL52"/>
-      <c r="AM52"/>
-      <c r="AN52" s="81"/>
-      <c r="AO52" s="82"/>
+      <c r="AL52" s="2"/>
+      <c r="AM52" s="2"/>
+      <c r="AN52" s="53"/>
+      <c r="AO52"/>
       <c r="AP52"/>
       <c r="AQ52"/>
       <c r="AR52" s="2"/>
@@ -13566,10 +13557,10 @@
       <c r="AT52" s="2"/>
       <c r="AU52"/>
       <c r="AV52"/>
-      <c r="AW52"/>
-      <c r="AX52"/>
-      <c r="AY52" s="81"/>
-      <c r="AZ52" s="82"/>
+      <c r="AW52" s="2"/>
+      <c r="AX52" s="2"/>
+      <c r="AY52" s="53"/>
+      <c r="AZ52"/>
       <c r="BA52"/>
       <c r="BB52"/>
       <c r="BC52" s="2"/>
@@ -13577,10 +13568,10 @@
       <c r="BE52" s="2"/>
       <c r="BF52"/>
       <c r="BG52"/>
-      <c r="BH52"/>
-      <c r="BI52"/>
-      <c r="BJ52" s="81"/>
-      <c r="BK52" s="82"/>
+      <c r="BH52" s="2"/>
+      <c r="BI52" s="2"/>
+      <c r="BJ52" s="53"/>
+      <c r="BK52"/>
       <c r="BL52"/>
       <c r="BM52"/>
       <c r="BN52" s="2"/>
@@ -13588,10 +13579,10 @@
       <c r="BP52" s="2"/>
       <c r="BQ52"/>
       <c r="BR52"/>
-      <c r="BS52"/>
-      <c r="BT52"/>
-      <c r="BU52" s="81"/>
-      <c r="BV52" s="82"/>
+      <c r="BS52" s="2"/>
+      <c r="BT52" s="2"/>
+      <c r="BU52" s="53"/>
+      <c r="BV52"/>
       <c r="BW52"/>
       <c r="BX52"/>
       <c r="BY52" s="2"/>
@@ -13599,10 +13590,10 @@
       <c r="CA52" s="2"/>
       <c r="CB52"/>
       <c r="CC52"/>
-      <c r="CD52"/>
-      <c r="CE52"/>
-      <c r="CF52" s="81"/>
-      <c r="CG52" s="82"/>
+      <c r="CD52" s="2"/>
+      <c r="CE52" s="2"/>
+      <c r="CF52" s="53"/>
+      <c r="CG52"/>
       <c r="CH52"/>
       <c r="CI52"/>
       <c r="CJ52" s="2"/>
@@ -13610,10 +13601,10 @@
       <c r="CL52" s="2"/>
       <c r="CM52"/>
       <c r="CN52"/>
-      <c r="CO52"/>
-      <c r="CP52"/>
-      <c r="CQ52" s="81"/>
-      <c r="CR52" s="82"/>
+      <c r="CO52" s="2"/>
+      <c r="CP52" s="2"/>
+      <c r="CQ52" s="53"/>
+      <c r="CR52"/>
       <c r="CS52"/>
       <c r="CT52"/>
       <c r="CU52" s="2"/>
@@ -13621,10 +13612,10 @@
       <c r="CW52" s="2"/>
       <c r="CX52"/>
       <c r="CY52"/>
-      <c r="CZ52"/>
-      <c r="DA52"/>
-      <c r="DB52" s="81"/>
-      <c r="DC52" s="82"/>
+      <c r="CZ52" s="2"/>
+      <c r="DA52" s="2"/>
+      <c r="DB52" s="53"/>
+      <c r="DC52"/>
       <c r="DD52"/>
       <c r="DE52"/>
       <c r="DF52" s="2"/>
@@ -13632,10 +13623,10 @@
       <c r="DH52" s="2"/>
       <c r="DI52"/>
       <c r="DJ52"/>
-      <c r="DK52"/>
-      <c r="DL52"/>
-      <c r="DM52" s="81"/>
-      <c r="DN52" s="82"/>
+      <c r="DK52" s="2"/>
+      <c r="DL52" s="2"/>
+      <c r="DM52" s="53"/>
+      <c r="DN52"/>
       <c r="DO52"/>
       <c r="DP52"/>
       <c r="DQ52" s="2"/>
@@ -13643,10 +13634,10 @@
       <c r="DS52" s="2"/>
       <c r="DT52"/>
       <c r="DU52"/>
-      <c r="DV52"/>
-      <c r="DW52"/>
+      <c r="DV52" s="2"/>
+      <c r="DW52" s="2"/>
     </row>
-    <row r="53" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="53" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="79"/>
       <c r="B53" s="79"/>
       <c r="C53" s="79"/>
@@ -13654,136 +13645,136 @@
       <c r="E53"/>
       <c r="F53" s="1"/>
       <c r="G53"/>
-      <c r="H53" s="82"/>
+      <c r="H53"/>
       <c r="I53"/>
-      <c r="J53" s="2"/>
+      <c r="J53"/>
       <c r="K53" s="2"/>
       <c r="L53"/>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
+      <c r="M53"/>
+      <c r="N53"/>
       <c r="O53"/>
       <c r="P53"/>
       <c r="Q53"/>
       <c r="R53"/>
-      <c r="S53" s="82"/>
+      <c r="S53"/>
       <c r="T53"/>
-      <c r="U53" s="2"/>
+      <c r="U53"/>
       <c r="V53" s="2"/>
       <c r="W53"/>
-      <c r="X53" s="2"/>
-      <c r="Y53" s="2"/>
+      <c r="X53"/>
+      <c r="Y53"/>
       <c r="Z53"/>
       <c r="AA53"/>
       <c r="AB53"/>
       <c r="AC53"/>
-      <c r="AD53" s="82"/>
+      <c r="AD53"/>
       <c r="AE53"/>
-      <c r="AF53" s="2"/>
+      <c r="AF53"/>
       <c r="AG53" s="2"/>
       <c r="AH53"/>
-      <c r="AI53" s="2"/>
-      <c r="AJ53" s="2"/>
+      <c r="AI53"/>
+      <c r="AJ53"/>
       <c r="AK53"/>
       <c r="AL53"/>
       <c r="AM53"/>
       <c r="AN53"/>
-      <c r="AO53" s="82"/>
+      <c r="AO53"/>
       <c r="AP53"/>
-      <c r="AQ53" s="2"/>
+      <c r="AQ53"/>
       <c r="AR53" s="2"/>
       <c r="AS53"/>
-      <c r="AT53" s="2"/>
-      <c r="AU53" s="2"/>
+      <c r="AT53"/>
+      <c r="AU53"/>
       <c r="AV53"/>
       <c r="AW53"/>
       <c r="AX53"/>
       <c r="AY53"/>
-      <c r="AZ53" s="82"/>
+      <c r="AZ53"/>
       <c r="BA53"/>
-      <c r="BB53" s="2"/>
+      <c r="BB53"/>
       <c r="BC53" s="2"/>
       <c r="BD53"/>
-      <c r="BE53" s="2"/>
-      <c r="BF53" s="2"/>
+      <c r="BE53"/>
+      <c r="BF53"/>
       <c r="BG53"/>
       <c r="BH53"/>
       <c r="BI53"/>
       <c r="BJ53"/>
-      <c r="BK53" s="82"/>
+      <c r="BK53"/>
       <c r="BL53"/>
-      <c r="BM53" s="2"/>
+      <c r="BM53"/>
       <c r="BN53" s="2"/>
       <c r="BO53"/>
-      <c r="BP53" s="2"/>
-      <c r="BQ53" s="2"/>
+      <c r="BP53"/>
+      <c r="BQ53"/>
       <c r="BR53"/>
       <c r="BS53"/>
       <c r="BT53"/>
       <c r="BU53"/>
-      <c r="BV53" s="82"/>
+      <c r="BV53"/>
       <c r="BW53"/>
-      <c r="BX53" s="2"/>
+      <c r="BX53"/>
       <c r="BY53" s="2"/>
       <c r="BZ53"/>
-      <c r="CA53" s="2"/>
-      <c r="CB53" s="2"/>
+      <c r="CA53"/>
+      <c r="CB53"/>
       <c r="CC53"/>
       <c r="CD53"/>
       <c r="CE53"/>
       <c r="CF53"/>
-      <c r="CG53" s="82"/>
+      <c r="CG53"/>
       <c r="CH53"/>
-      <c r="CI53" s="2"/>
+      <c r="CI53"/>
       <c r="CJ53" s="2"/>
       <c r="CK53"/>
-      <c r="CL53" s="2"/>
-      <c r="CM53" s="2"/>
+      <c r="CL53"/>
+      <c r="CM53"/>
       <c r="CN53"/>
       <c r="CO53"/>
       <c r="CP53"/>
       <c r="CQ53"/>
-      <c r="CR53" s="82"/>
+      <c r="CR53"/>
       <c r="CS53"/>
-      <c r="CT53" s="2"/>
+      <c r="CT53"/>
       <c r="CU53" s="2"/>
       <c r="CV53"/>
-      <c r="CW53" s="2"/>
-      <c r="CX53" s="2"/>
+      <c r="CW53"/>
+      <c r="CX53"/>
       <c r="CY53"/>
       <c r="CZ53"/>
       <c r="DA53"/>
       <c r="DB53"/>
-      <c r="DC53" s="82"/>
+      <c r="DC53"/>
       <c r="DD53"/>
-      <c r="DE53" s="2"/>
-      <c r="DF53" s="2"/>
+      <c r="DE53"/>
+      <c r="DF53"/>
       <c r="DG53"/>
-      <c r="DH53" s="2"/>
-      <c r="DI53" s="2"/>
+      <c r="DH53"/>
+      <c r="DI53"/>
       <c r="DJ53"/>
       <c r="DK53"/>
       <c r="DL53"/>
       <c r="DM53"/>
-      <c r="DN53" s="82"/>
+      <c r="DN53"/>
       <c r="DO53"/>
-      <c r="DP53" s="2"/>
+      <c r="DP53"/>
       <c r="DQ53" s="2"/>
       <c r="DR53"/>
-      <c r="DS53" s="2"/>
-      <c r="DT53" s="2"/>
+      <c r="DS53"/>
+      <c r="DT53"/>
       <c r="DU53"/>
       <c r="DV53"/>
       <c r="DW53"/>
     </row>
-    <row r="54" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="54" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="79"/>
       <c r="B54" s="79"/>
       <c r="C54" s="79"/>
       <c r="D54" s="80"/>
       <c r="E54"/>
       <c r="F54" s="1"/>
-      <c r="G54"/>
-      <c r="H54" s="82"/>
+      <c r="G54" s="53"/>
+      <c r="H54"/>
       <c r="I54"/>
       <c r="J54"/>
       <c r="K54" s="2"/>
@@ -13793,8 +13784,8 @@
       <c r="O54"/>
       <c r="P54"/>
       <c r="Q54"/>
-      <c r="R54"/>
-      <c r="S54" s="82"/>
+      <c r="R54" s="53"/>
+      <c r="S54"/>
       <c r="T54"/>
       <c r="U54"/>
       <c r="V54" s="2"/>
@@ -13804,8 +13795,8 @@
       <c r="Z54"/>
       <c r="AA54"/>
       <c r="AB54"/>
-      <c r="AC54"/>
-      <c r="AD54" s="82"/>
+      <c r="AC54" s="53"/>
+      <c r="AD54"/>
       <c r="AE54"/>
       <c r="AF54"/>
       <c r="AG54" s="2"/>
@@ -13815,8 +13806,8 @@
       <c r="AK54"/>
       <c r="AL54"/>
       <c r="AM54"/>
-      <c r="AN54"/>
-      <c r="AO54" s="82"/>
+      <c r="AN54" s="53"/>
+      <c r="AO54"/>
       <c r="AP54"/>
       <c r="AQ54"/>
       <c r="AR54" s="2"/>
@@ -13826,8 +13817,8 @@
       <c r="AV54"/>
       <c r="AW54"/>
       <c r="AX54"/>
-      <c r="AY54"/>
-      <c r="AZ54" s="82"/>
+      <c r="AY54" s="53"/>
+      <c r="AZ54"/>
       <c r="BA54"/>
       <c r="BB54"/>
       <c r="BC54" s="2"/>
@@ -13837,8 +13828,8 @@
       <c r="BG54"/>
       <c r="BH54"/>
       <c r="BI54"/>
-      <c r="BJ54"/>
-      <c r="BK54" s="82"/>
+      <c r="BJ54" s="53"/>
+      <c r="BK54"/>
       <c r="BL54"/>
       <c r="BM54"/>
       <c r="BN54" s="2"/>
@@ -13848,8 +13839,8 @@
       <c r="BR54"/>
       <c r="BS54"/>
       <c r="BT54"/>
-      <c r="BU54"/>
-      <c r="BV54" s="82"/>
+      <c r="BU54" s="53"/>
+      <c r="BV54"/>
       <c r="BW54"/>
       <c r="BX54"/>
       <c r="BY54" s="2"/>
@@ -13859,8 +13850,8 @@
       <c r="CC54"/>
       <c r="CD54"/>
       <c r="CE54"/>
-      <c r="CF54"/>
-      <c r="CG54" s="82"/>
+      <c r="CF54" s="53"/>
+      <c r="CG54"/>
       <c r="CH54"/>
       <c r="CI54"/>
       <c r="CJ54" s="2"/>
@@ -13870,8 +13861,8 @@
       <c r="CN54"/>
       <c r="CO54"/>
       <c r="CP54"/>
-      <c r="CQ54"/>
-      <c r="CR54" s="82"/>
+      <c r="CQ54" s="53"/>
+      <c r="CR54"/>
       <c r="CS54"/>
       <c r="CT54"/>
       <c r="CU54" s="2"/>
@@ -13881,19 +13872,19 @@
       <c r="CY54"/>
       <c r="CZ54"/>
       <c r="DA54"/>
-      <c r="DB54"/>
-      <c r="DC54" s="82"/>
-      <c r="DD54"/>
-      <c r="DE54"/>
-      <c r="DF54" s="2"/>
-      <c r="DG54"/>
-      <c r="DH54"/>
+      <c r="DB54" s="53"/>
+      <c r="DC54" s="53"/>
+      <c r="DD54" s="53"/>
+      <c r="DE54" s="53"/>
+      <c r="DF54" s="53"/>
+      <c r="DG54" s="53"/>
+      <c r="DH54" s="53"/>
       <c r="DI54"/>
       <c r="DJ54"/>
       <c r="DK54"/>
       <c r="DL54"/>
-      <c r="DM54"/>
-      <c r="DN54" s="82"/>
+      <c r="DM54" s="53"/>
+      <c r="DN54"/>
       <c r="DO54"/>
       <c r="DP54"/>
       <c r="DQ54" s="2"/>
@@ -13904,1238 +13895,27 @@
       <c r="DV54"/>
       <c r="DW54"/>
     </row>
-    <row r="55" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="55" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A55" s="79"/>
       <c r="B55" s="79"/>
       <c r="C55" s="79"/>
       <c r="D55" s="80"/>
-      <c r="E55"/>
-      <c r="F55" s="1"/>
-      <c r="G55" s="53">
-        <v>40908</v>
-      </c>
-      <c r="H55" s="57">
-        <v>24.4</v>
-      </c>
-      <c r="I55" s="83">
-        <v>14.896780080660626</v>
-      </c>
-      <c r="K55" s="58"/>
-      <c r="M55" s="78">
-        <v>-363.48143396811923</v>
-      </c>
-      <c r="N55" s="84">
-        <v>49.649661270000003</v>
-      </c>
-      <c r="O55" s="78">
-        <v>-564.15953366191786</v>
-      </c>
-      <c r="P55" s="78">
-        <v>-18046.730074450992</v>
-      </c>
-      <c r="Q55" s="78"/>
-      <c r="R55" s="53">
-        <v>40908</v>
-      </c>
-      <c r="S55" s="57">
-        <v>2.17</v>
-      </c>
-      <c r="T55" s="83">
-        <v>514.67011145940978</v>
-      </c>
-      <c r="V55" s="58"/>
-      <c r="X55" s="78">
-        <v>-1116.8341418669193</v>
-      </c>
-      <c r="Y55" s="84">
-        <v>49.649661270000003</v>
-      </c>
-      <c r="Z55" s="78">
-        <v>-1733.4382715916454</v>
-      </c>
-      <c r="AA55" s="78">
-        <v>-55450.436838463669</v>
-      </c>
-      <c r="AB55" s="78"/>
-      <c r="AC55" s="53">
-        <v>40908</v>
-      </c>
-      <c r="AD55" s="57">
-        <v>1.2</v>
-      </c>
-      <c r="AE55" s="83">
-        <v>315.91124093442238</v>
-      </c>
-      <c r="AG55" s="58"/>
-      <c r="AI55" s="78">
-        <v>-379.09348912130685</v>
-      </c>
-      <c r="AJ55" s="84">
-        <v>49.649661270000003</v>
-      </c>
-      <c r="AK55" s="78">
-        <v>-588.39100446518034</v>
-      </c>
-      <c r="AL55" s="78">
-        <v>-18821.863324535316</v>
-      </c>
-      <c r="AM55" s="78"/>
-      <c r="AN55" s="53">
-        <v>40908</v>
-      </c>
-      <c r="AO55" s="57">
-        <v>4.13</v>
-      </c>
-      <c r="AP55" s="83">
-        <v>163.57279842571759</v>
-      </c>
-      <c r="AR55" s="58"/>
-      <c r="AT55" s="78">
-        <v>-675.55565749821369</v>
-      </c>
-      <c r="AU55" s="84">
-        <v>49.649661270000003</v>
-      </c>
-      <c r="AV55" s="78">
-        <v>-1048.5299360029776</v>
-      </c>
-      <c r="AW55" s="78">
-        <v>-33541.109563818449</v>
-      </c>
-      <c r="AX55" s="78"/>
-      <c r="AY55" s="53">
-        <v>40908</v>
-      </c>
-      <c r="AZ55" s="57">
-        <v>347.46</v>
-      </c>
-      <c r="BA55" s="83">
-        <v>3.4933407096887072</v>
-      </c>
-      <c r="BC55" s="58"/>
-      <c r="BE55" s="78">
-        <v>-1213.7961629884383</v>
-      </c>
-      <c r="BF55" s="84">
-        <v>49.649661270000003</v>
-      </c>
-      <c r="BG55" s="78">
-        <v>-1883.9330245743552</v>
-      </c>
-      <c r="BH55" s="78">
-        <v>-60264.568343201674</v>
-      </c>
-      <c r="BI55" s="78"/>
-      <c r="BJ55" s="53">
-        <v>40908</v>
-      </c>
-      <c r="BK55" s="57">
-        <v>2.5299999999999998</v>
-      </c>
-      <c r="BL55" s="83">
-        <v>349.68974518100589</v>
-      </c>
-      <c r="BN55" s="58"/>
-      <c r="BP55" s="78">
-        <v>-884.71505530794479</v>
-      </c>
-      <c r="BQ55" s="84">
-        <v>49.649661270000003</v>
-      </c>
-      <c r="BR55" s="78">
-        <v>-1373.166237343461</v>
-      </c>
-      <c r="BS55" s="78">
-        <v>-43925.802816508774</v>
-      </c>
-      <c r="BT55" s="78"/>
-      <c r="BU55" s="53">
-        <v>40908</v>
-      </c>
-      <c r="BV55" s="57">
-        <v>1.56</v>
-      </c>
-      <c r="BW55" s="83">
-        <v>504.35786333466439</v>
-      </c>
-      <c r="BY55" s="58"/>
-      <c r="CA55" s="78">
-        <v>-786.79826680207645</v>
-      </c>
-      <c r="CB55" s="84">
-        <v>49.649661270000003</v>
-      </c>
-      <c r="CC55" s="78">
-        <v>-1221.1895899035028</v>
-      </c>
-      <c r="CD55" s="78">
-        <v>-39064.267434546186</v>
-      </c>
-      <c r="CE55" s="78"/>
-      <c r="CF55" s="53">
-        <v>40908</v>
-      </c>
-      <c r="CG55" s="57">
-        <v>250.73</v>
-      </c>
-      <c r="CH55" s="83">
-        <v>1.5555028182374608</v>
-      </c>
-      <c r="CJ55" s="58"/>
-      <c r="CL55" s="78">
-        <v>-390.01122161667854</v>
-      </c>
-      <c r="CM55" s="84">
-        <v>49.649661270000003</v>
-      </c>
-      <c r="CN55" s="78">
-        <v>-605.33641707124673</v>
-      </c>
-      <c r="CO55" s="78">
-        <v>-19363.925044766991</v>
-      </c>
-      <c r="CP55" s="78"/>
-      <c r="CQ55" s="53">
-        <v>40908</v>
-      </c>
-      <c r="CR55" s="57">
-        <v>8.7899999999999991</v>
-      </c>
-      <c r="CS55" s="83">
-        <v>40.25869578250672</v>
-      </c>
-      <c r="CU55" s="58"/>
-      <c r="CW55" s="78">
-        <v>-353.87393592823406</v>
-      </c>
-      <c r="CX55" s="84">
-        <v>49.649661270000003</v>
-      </c>
-      <c r="CY55" s="78">
-        <v>-549.24773595421209</v>
-      </c>
-      <c r="CZ55" s="78">
-        <v>-17569.721051118504</v>
-      </c>
-      <c r="DA55" s="78"/>
-      <c r="DB55" s="53">
-        <v>40908</v>
-      </c>
-      <c r="DC55" s="57">
-        <v>237</v>
-      </c>
-      <c r="DD55" s="83">
-        <v>1.556164507017314</v>
-      </c>
-      <c r="DF55" s="58"/>
-      <c r="DH55" s="78">
-        <v>-368.81098816310345</v>
-      </c>
-      <c r="DI55" s="84">
-        <v>49.649661270000003</v>
-      </c>
-      <c r="DJ55" s="78">
-        <v>-572.43153472795291</v>
-      </c>
-      <c r="DK55" s="78">
-        <v>-18311.340634952066</v>
-      </c>
-      <c r="DL55" s="78"/>
-      <c r="DM55" s="53">
-        <v>40908</v>
-      </c>
-      <c r="DN55" s="57">
-        <v>491.94</v>
-      </c>
-      <c r="DO55" s="83">
-        <v>2.3749276978677343</v>
-      </c>
-      <c r="DQ55" s="58"/>
-      <c r="DS55" s="78">
-        <v>-1168.3219316890531</v>
-      </c>
-      <c r="DT55" s="84">
-        <v>49.649661270000003</v>
-      </c>
-      <c r="DU55" s="78">
-        <v>-1813.3524701745794</v>
-      </c>
-      <c r="DV55" s="78">
-        <v>-58006.788162673569</v>
-      </c>
-      <c r="DW55" s="78"/>
     </row>
-    <row r="56" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
+    <row r="56" spans="1:127" x14ac:dyDescent="0.25">
       <c r="A56" s="79"/>
       <c r="B56" s="79"/>
       <c r="C56" s="79"/>
-      <c r="D56" s="80"/>
-      <c r="E56"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="53">
-        <v>40918</v>
-      </c>
-      <c r="H56"/>
-      <c r="I56"/>
-      <c r="J56"/>
-      <c r="K56" s="2"/>
-      <c r="L56"/>
-      <c r="M56" s="78">
-        <v>-15.004688965301655</v>
-      </c>
-      <c r="N56" s="78"/>
-      <c r="O56" s="78">
-        <v>-23.225758049390432</v>
-      </c>
-      <c r="P56" s="78">
-        <v>-732.7773116098781</v>
-      </c>
-      <c r="Q56" s="78"/>
-      <c r="R56" s="53">
-        <v>40918</v>
-      </c>
-      <c r="S56"/>
-      <c r="T56"/>
-      <c r="U56"/>
-      <c r="V56" s="2"/>
-      <c r="W56"/>
-      <c r="X56" s="78">
-        <v>-45.014066895904975</v>
-      </c>
-      <c r="Y56" s="78"/>
-      <c r="Z56" s="78">
-        <v>-69.677274148171307</v>
-      </c>
-      <c r="AA56" s="78">
-        <v>-2198.3319348296345</v>
-      </c>
-      <c r="AB56" s="78"/>
-      <c r="AC56" s="53">
-        <v>40918</v>
-      </c>
-      <c r="AD56"/>
-      <c r="AE56"/>
-      <c r="AF56"/>
-      <c r="AG56" s="2"/>
-      <c r="AH56"/>
-      <c r="AI56" s="78">
-        <v>-15.004688965301657</v>
-      </c>
-      <c r="AJ56" s="78"/>
-      <c r="AK56" s="78">
-        <v>-23.225758049390436</v>
-      </c>
-      <c r="AL56" s="78">
-        <v>-732.77731160987821</v>
-      </c>
-      <c r="AM56" s="78"/>
-      <c r="AN56" s="53">
-        <v>40918</v>
-      </c>
-      <c r="AO56"/>
-      <c r="AP56"/>
-      <c r="AQ56"/>
-      <c r="AR56" s="2"/>
-      <c r="AS56"/>
-      <c r="AT56" s="78">
-        <v>-29.9781181619256</v>
-      </c>
-      <c r="AU56" s="78"/>
-      <c r="AV56" s="78">
-        <v>-46.403129102844638</v>
-      </c>
-      <c r="AW56" s="78">
-        <v>-1464.028003820569</v>
-      </c>
-      <c r="AX56" s="78"/>
-      <c r="AY56" s="53">
-        <v>40918</v>
-      </c>
-      <c r="AZ56"/>
-      <c r="BA56"/>
-      <c r="BB56"/>
-      <c r="BC56" s="2"/>
-      <c r="BD56"/>
-      <c r="BE56" s="78">
-        <v>-45.014066895904975</v>
-      </c>
-      <c r="BF56" s="78"/>
-      <c r="BG56" s="78">
-        <v>-69.677274148171307</v>
-      </c>
-      <c r="BH56" s="78">
-        <v>-2198.3319348296345</v>
-      </c>
-      <c r="BI56" s="78"/>
-      <c r="BJ56" s="53">
-        <v>40918</v>
-      </c>
-      <c r="BK56"/>
-      <c r="BL56"/>
-      <c r="BM56"/>
-      <c r="BN56" s="2"/>
-      <c r="BO56"/>
-      <c r="BP56" s="78">
-        <v>-29.9781181619256</v>
-      </c>
-      <c r="BQ56" s="78"/>
-      <c r="BR56" s="78">
-        <v>-46.403129102844638</v>
-      </c>
-      <c r="BS56" s="78">
-        <v>-1464.028003820569</v>
-      </c>
-      <c r="BT56" s="78"/>
-      <c r="BU56" s="53">
-        <v>40918</v>
-      </c>
-      <c r="BV56"/>
-      <c r="BW56"/>
-      <c r="BX56"/>
-      <c r="BY56" s="2"/>
-      <c r="BZ56"/>
-      <c r="CA56" s="78">
-        <v>-29.978118161925604</v>
-      </c>
-      <c r="CB56" s="78"/>
-      <c r="CC56" s="78">
-        <v>-46.403129102844645</v>
-      </c>
-      <c r="CD56" s="78">
-        <v>-1464.0280038205692</v>
-      </c>
-      <c r="CE56" s="78"/>
-      <c r="CF56" s="53">
-        <v>40918</v>
-      </c>
-      <c r="CG56"/>
-      <c r="CH56"/>
-      <c r="CI56"/>
-      <c r="CJ56" s="2"/>
-      <c r="CK56"/>
-      <c r="CL56" s="78">
-        <v>-15.004688965301657</v>
-      </c>
-      <c r="CM56" s="78"/>
-      <c r="CN56" s="78">
-        <v>-23.225758049390436</v>
-      </c>
-      <c r="CO56" s="78">
-        <v>-732.77731160987821</v>
-      </c>
-      <c r="CP56" s="78"/>
-      <c r="CQ56" s="53">
-        <v>40918</v>
-      </c>
-      <c r="CR56"/>
-      <c r="CS56"/>
-      <c r="CT56"/>
-      <c r="CU56" s="2"/>
-      <c r="CV56"/>
-      <c r="CW56" s="78">
-        <v>-15.004688965301657</v>
-      </c>
-      <c r="CX56" s="78"/>
-      <c r="CY56" s="78">
-        <v>-23.225758049390436</v>
-      </c>
-      <c r="CZ56" s="78">
-        <v>-732.77731160987821</v>
-      </c>
-      <c r="DA56" s="78"/>
-      <c r="DB56" s="53">
-        <v>40918</v>
-      </c>
-      <c r="DC56"/>
-      <c r="DD56"/>
-      <c r="DE56"/>
-      <c r="DF56" s="2"/>
-      <c r="DG56"/>
-      <c r="DH56" s="78">
-        <v>-15.004688965301659</v>
-      </c>
-      <c r="DI56" s="78"/>
-      <c r="DJ56" s="78">
-        <v>-23.225758049390439</v>
-      </c>
-      <c r="DK56" s="78">
-        <v>-732.77731160987821</v>
-      </c>
-      <c r="DL56" s="78"/>
-      <c r="DM56" s="53">
-        <v>40918</v>
-      </c>
-      <c r="DN56"/>
-      <c r="DO56"/>
-      <c r="DP56"/>
-      <c r="DQ56" s="2"/>
-      <c r="DR56"/>
-      <c r="DS56" s="78">
-        <v>-45.014066895904975</v>
-      </c>
-      <c r="DT56" s="78"/>
-      <c r="DU56" s="78">
-        <v>-69.677274148171307</v>
-      </c>
-      <c r="DV56" s="78">
-        <v>-2198.3319348296345</v>
-      </c>
-      <c r="DW56" s="78"/>
-    </row>
-    <row r="57" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A57" s="79"/>
-      <c r="B57" s="79"/>
-      <c r="C57" s="79"/>
-      <c r="D57" s="80"/>
-      <c r="E57"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="53">
-        <v>41110</v>
-      </c>
-      <c r="H57"/>
-      <c r="I57"/>
-      <c r="J57"/>
-      <c r="K57" s="2"/>
-      <c r="L57"/>
-      <c r="M57" s="2">
-        <v>382.36405452085353</v>
-      </c>
-      <c r="N57"/>
-      <c r="O57" s="78">
-        <v>597.21441675612118</v>
-      </c>
-      <c r="P57" s="2">
-        <v>19115.519608646577</v>
-      </c>
-      <c r="Q57" s="2"/>
-      <c r="R57" s="53">
-        <v>41110</v>
-      </c>
-      <c r="S57"/>
-      <c r="T57"/>
-      <c r="U57"/>
-      <c r="V57" s="2"/>
-      <c r="W57"/>
-      <c r="X57" s="2">
-        <v>1199.3271832390444</v>
-      </c>
-      <c r="Y57"/>
-      <c r="Z57" s="78">
-        <v>1873.2291275010637</v>
-      </c>
-      <c r="AA57" s="2">
-        <v>59957.943267228547</v>
-      </c>
-      <c r="AB57" s="2"/>
-      <c r="AC57" s="53">
-        <v>41110</v>
-      </c>
-      <c r="AD57"/>
-      <c r="AE57"/>
-      <c r="AF57"/>
-      <c r="AG57" s="2"/>
-      <c r="AH57"/>
-      <c r="AI57" s="2">
-        <v>433.50799589526935</v>
-      </c>
-      <c r="AJ57"/>
-      <c r="AK57" s="78">
-        <v>677.09613878882124</v>
-      </c>
-      <c r="AL57" s="2">
-        <v>21672.357791124836</v>
-      </c>
-      <c r="AM57" s="2"/>
-      <c r="AN57" s="53">
-        <v>41110</v>
-      </c>
-      <c r="AO57"/>
-      <c r="AP57"/>
-      <c r="AQ57"/>
-      <c r="AR57" s="2"/>
-      <c r="AS57"/>
-      <c r="AT57" s="2">
-        <v>700.40883297979917</v>
-      </c>
-      <c r="AU57"/>
-      <c r="AV57" s="78">
-        <v>1093.9685562311483</v>
-      </c>
-      <c r="AW57" s="2">
-        <v>35015.526754135353</v>
-      </c>
-      <c r="AX57" s="2"/>
-      <c r="AY57" s="53">
-        <v>41110</v>
-      </c>
-      <c r="AZ57"/>
-      <c r="BA57"/>
-      <c r="BB57"/>
-      <c r="BC57" s="2"/>
-      <c r="BD57"/>
-      <c r="BE57" s="2">
-        <v>1337.4269972489039</v>
-      </c>
-      <c r="BF57"/>
-      <c r="BG57" s="78">
-        <v>2088.9272270030633</v>
-      </c>
-      <c r="BH57" s="2">
-        <v>66861.964896468649</v>
-      </c>
-      <c r="BI57" s="2"/>
-      <c r="BJ57" s="53">
-        <v>41110</v>
-      </c>
-      <c r="BK57"/>
-      <c r="BL57"/>
-      <c r="BM57"/>
-      <c r="BN57" s="2"/>
-      <c r="BO57"/>
-      <c r="BP57" s="2">
-        <v>903.84700935757951</v>
-      </c>
-      <c r="BQ57"/>
-      <c r="BR57" s="78">
-        <v>1411.7186439156035</v>
-      </c>
-      <c r="BS57" s="2">
-        <v>45186.00801072186</v>
-      </c>
-      <c r="BT57" s="2"/>
-      <c r="BU57" s="53">
-        <v>41110</v>
-      </c>
-      <c r="BV57"/>
-      <c r="BW57"/>
-      <c r="BX57"/>
-      <c r="BY57" s="2"/>
-      <c r="BZ57"/>
-      <c r="CA57" s="2">
-        <v>827.24787707892517</v>
-      </c>
-      <c r="CB57"/>
-      <c r="CC57" s="78">
-        <v>1292.0784592095733</v>
-      </c>
-      <c r="CD57" s="2">
-        <v>41356.588906688186</v>
-      </c>
-      <c r="CE57" s="2"/>
-      <c r="CF57" s="53">
-        <v>41110</v>
-      </c>
-      <c r="CG57"/>
-      <c r="CH57"/>
-      <c r="CI57"/>
-      <c r="CJ57" s="2"/>
-      <c r="CK57"/>
-      <c r="CL57" s="2">
-        <v>409.87810453903268</v>
-      </c>
-      <c r="CM57"/>
-      <c r="CN57" s="78">
-        <v>640.1886114795152</v>
-      </c>
-      <c r="CO57" s="2">
-        <v>20491.029038514029</v>
-      </c>
-      <c r="CP57" s="2"/>
-      <c r="CQ57" s="53">
-        <v>41110</v>
-      </c>
-      <c r="CR57"/>
-      <c r="CS57"/>
-      <c r="CT57"/>
-      <c r="CU57" s="2"/>
-      <c r="CV57"/>
-      <c r="CW57" s="2">
-        <v>292.5010256550562</v>
-      </c>
-      <c r="CX57"/>
-      <c r="CY57" s="78">
-        <v>456.85735197063229</v>
-      </c>
-      <c r="CZ57" s="2">
-        <v>14622.998750405606</v>
-      </c>
-      <c r="DA57" s="2"/>
-      <c r="DB57" s="53">
-        <v>41110</v>
-      </c>
-      <c r="DC57"/>
-      <c r="DD57"/>
-      <c r="DE57"/>
-      <c r="DF57" s="2"/>
-      <c r="DG57"/>
-      <c r="DH57" s="2">
-        <v>349.40182422132233</v>
-      </c>
-      <c r="DI57"/>
-      <c r="DJ57" s="78">
-        <v>545.73070925128332</v>
-      </c>
-      <c r="DK57" s="2">
-        <v>17467.639395573231</v>
-      </c>
-      <c r="DL57" s="2"/>
-      <c r="DM57" s="53">
-        <v>41110</v>
-      </c>
-      <c r="DN57"/>
-      <c r="DO57"/>
-      <c r="DP57"/>
-      <c r="DQ57" s="2"/>
-      <c r="DR57"/>
-      <c r="DS57" s="2">
-        <v>1282.0507624191184</v>
-      </c>
-      <c r="DT57"/>
-      <c r="DU57" s="78">
-        <v>2002.4350858224211</v>
-      </c>
-      <c r="DV57" s="2">
-        <v>64093.541739986904</v>
-      </c>
-      <c r="DW57" s="2"/>
-    </row>
-    <row r="58" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="79"/>
-      <c r="B58" s="79"/>
-      <c r="C58" s="79"/>
-      <c r="D58" s="80"/>
-      <c r="E58"/>
-      <c r="F58" s="1"/>
-      <c r="G58" s="53"/>
-      <c r="H58"/>
-      <c r="I58"/>
-      <c r="J58"/>
-      <c r="K58" s="2"/>
-      <c r="L58"/>
-      <c r="M58" s="2"/>
-      <c r="N58"/>
-      <c r="O58"/>
-      <c r="P58" s="2"/>
-      <c r="Q58" s="2"/>
-      <c r="R58" s="53"/>
-      <c r="S58"/>
-      <c r="T58"/>
-      <c r="U58"/>
-      <c r="V58" s="2"/>
-      <c r="W58"/>
-      <c r="X58" s="2"/>
-      <c r="Y58"/>
-      <c r="Z58"/>
-      <c r="AA58" s="2"/>
-      <c r="AB58" s="2"/>
-      <c r="AC58" s="53"/>
-      <c r="AD58"/>
-      <c r="AE58"/>
-      <c r="AF58"/>
-      <c r="AG58" s="2"/>
-      <c r="AH58"/>
-      <c r="AI58" s="2"/>
-      <c r="AJ58"/>
-      <c r="AK58"/>
-      <c r="AL58" s="2"/>
-      <c r="AM58" s="2"/>
-      <c r="AN58" s="53"/>
-      <c r="AO58"/>
-      <c r="AP58"/>
-      <c r="AQ58"/>
-      <c r="AR58" s="2"/>
-      <c r="AS58"/>
-      <c r="AT58" s="2"/>
-      <c r="AU58"/>
-      <c r="AV58"/>
-      <c r="AW58" s="2"/>
-      <c r="AX58" s="2"/>
-      <c r="AY58" s="53"/>
-      <c r="AZ58"/>
-      <c r="BA58"/>
-      <c r="BB58"/>
-      <c r="BC58" s="2"/>
-      <c r="BD58"/>
-      <c r="BE58" s="2"/>
-      <c r="BF58"/>
-      <c r="BG58"/>
-      <c r="BH58" s="2"/>
-      <c r="BI58" s="2"/>
-      <c r="BJ58" s="53"/>
-      <c r="BK58"/>
-      <c r="BL58"/>
-      <c r="BM58"/>
-      <c r="BN58" s="2"/>
-      <c r="BO58"/>
-      <c r="BP58" s="2"/>
-      <c r="BQ58"/>
-      <c r="BR58"/>
-      <c r="BS58" s="2"/>
-      <c r="BT58" s="2"/>
-      <c r="BU58" s="53"/>
-      <c r="BV58"/>
-      <c r="BW58"/>
-      <c r="BX58"/>
-      <c r="BY58" s="2"/>
-      <c r="BZ58"/>
-      <c r="CA58" s="2"/>
-      <c r="CB58"/>
-      <c r="CC58"/>
-      <c r="CD58" s="2"/>
-      <c r="CE58" s="2"/>
-      <c r="CF58" s="53"/>
-      <c r="CG58"/>
-      <c r="CH58"/>
-      <c r="CI58"/>
-      <c r="CJ58" s="2"/>
-      <c r="CK58"/>
-      <c r="CL58" s="2"/>
-      <c r="CM58"/>
-      <c r="CN58"/>
-      <c r="CO58" s="2"/>
-      <c r="CP58" s="2"/>
-      <c r="CQ58" s="53"/>
-      <c r="CR58"/>
-      <c r="CS58"/>
-      <c r="CT58"/>
-      <c r="CU58" s="2"/>
-      <c r="CV58"/>
-      <c r="CW58" s="2"/>
-      <c r="CX58"/>
-      <c r="CY58"/>
-      <c r="CZ58" s="2"/>
-      <c r="DA58" s="2"/>
-      <c r="DB58" s="53"/>
-      <c r="DC58"/>
-      <c r="DD58"/>
-      <c r="DE58"/>
-      <c r="DF58" s="2"/>
-      <c r="DG58"/>
-      <c r="DH58" s="2"/>
-      <c r="DI58"/>
-      <c r="DJ58"/>
-      <c r="DK58" s="2"/>
-      <c r="DL58" s="2"/>
-      <c r="DM58" s="53"/>
-      <c r="DN58"/>
-      <c r="DO58"/>
-      <c r="DP58"/>
-      <c r="DQ58" s="2"/>
-      <c r="DR58"/>
-      <c r="DS58" s="2"/>
-      <c r="DT58"/>
-      <c r="DU58"/>
-      <c r="DV58" s="2"/>
-      <c r="DW58" s="2"/>
-    </row>
-    <row r="59" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="79"/>
-      <c r="B59" s="79"/>
-      <c r="C59" s="79"/>
-      <c r="D59" s="80"/>
-      <c r="E59"/>
-      <c r="F59" s="1"/>
-      <c r="G59" s="53"/>
-      <c r="H59"/>
-      <c r="I59"/>
-      <c r="J59"/>
-      <c r="K59" s="2"/>
-      <c r="L59"/>
-      <c r="M59" s="2"/>
-      <c r="N59"/>
-      <c r="O59"/>
-      <c r="P59" s="2"/>
-      <c r="Q59" s="2"/>
-      <c r="R59" s="53"/>
-      <c r="S59"/>
-      <c r="T59"/>
-      <c r="U59"/>
-      <c r="V59" s="2"/>
-      <c r="W59"/>
-      <c r="X59" s="2"/>
-      <c r="Y59"/>
-      <c r="Z59"/>
-      <c r="AA59" s="2"/>
-      <c r="AB59" s="2"/>
-      <c r="AC59" s="53"/>
-      <c r="AD59"/>
-      <c r="AE59"/>
-      <c r="AF59"/>
-      <c r="AG59" s="2"/>
-      <c r="AH59"/>
-      <c r="AI59" s="2"/>
-      <c r="AJ59"/>
-      <c r="AK59"/>
-      <c r="AL59" s="2"/>
-      <c r="AM59" s="2"/>
-      <c r="AN59" s="53"/>
-      <c r="AO59"/>
-      <c r="AP59"/>
-      <c r="AQ59"/>
-      <c r="AR59" s="2"/>
-      <c r="AS59"/>
-      <c r="AT59" s="2"/>
-      <c r="AU59"/>
-      <c r="AV59"/>
-      <c r="AW59" s="2"/>
-      <c r="AX59" s="2"/>
-      <c r="AY59" s="53"/>
-      <c r="AZ59"/>
-      <c r="BA59"/>
-      <c r="BB59"/>
-      <c r="BC59" s="2"/>
-      <c r="BD59"/>
-      <c r="BE59" s="2"/>
-      <c r="BF59"/>
-      <c r="BG59"/>
-      <c r="BH59" s="2"/>
-      <c r="BI59" s="2"/>
-      <c r="BJ59" s="53"/>
-      <c r="BK59"/>
-      <c r="BL59"/>
-      <c r="BM59"/>
-      <c r="BN59" s="2"/>
-      <c r="BO59"/>
-      <c r="BP59" s="2"/>
-      <c r="BQ59"/>
-      <c r="BR59"/>
-      <c r="BS59" s="2"/>
-      <c r="BT59" s="2"/>
-      <c r="BU59" s="53"/>
-      <c r="BV59"/>
-      <c r="BW59"/>
-      <c r="BX59"/>
-      <c r="BY59" s="2"/>
-      <c r="BZ59"/>
-      <c r="CA59" s="2"/>
-      <c r="CB59"/>
-      <c r="CC59"/>
-      <c r="CD59" s="2"/>
-      <c r="CE59" s="2"/>
-      <c r="CF59" s="53"/>
-      <c r="CG59"/>
-      <c r="CH59"/>
-      <c r="CI59"/>
-      <c r="CJ59" s="2"/>
-      <c r="CK59"/>
-      <c r="CL59" s="2"/>
-      <c r="CM59"/>
-      <c r="CN59"/>
-      <c r="CO59" s="2"/>
-      <c r="CP59" s="2"/>
-      <c r="CQ59" s="53"/>
-      <c r="CR59"/>
-      <c r="CS59"/>
-      <c r="CT59"/>
-      <c r="CU59" s="2"/>
-      <c r="CV59"/>
-      <c r="CW59" s="2"/>
-      <c r="CX59"/>
-      <c r="CY59"/>
-      <c r="CZ59" s="2"/>
-      <c r="DA59" s="2"/>
-      <c r="DB59" s="53"/>
-      <c r="DC59"/>
-      <c r="DD59"/>
-      <c r="DE59"/>
-      <c r="DF59" s="2"/>
-      <c r="DG59"/>
-      <c r="DH59" s="2"/>
-      <c r="DI59"/>
-      <c r="DJ59"/>
-      <c r="DK59" s="2"/>
-      <c r="DL59" s="2"/>
-      <c r="DM59" s="53"/>
-      <c r="DN59"/>
-      <c r="DO59"/>
-      <c r="DP59"/>
-      <c r="DQ59" s="2"/>
-      <c r="DR59"/>
-      <c r="DS59" s="2"/>
-      <c r="DT59"/>
-      <c r="DU59"/>
-      <c r="DV59" s="2"/>
-      <c r="DW59" s="2"/>
-    </row>
-    <row r="60" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A60" s="79"/>
-      <c r="B60" s="79"/>
-      <c r="C60" s="79"/>
-      <c r="D60" s="80"/>
-      <c r="E60"/>
-      <c r="F60" s="1"/>
-      <c r="G60"/>
-      <c r="H60"/>
-      <c r="I60"/>
-      <c r="J60"/>
-      <c r="K60" s="2"/>
-      <c r="L60"/>
-      <c r="M60"/>
-      <c r="N60"/>
-      <c r="O60"/>
-      <c r="P60"/>
-      <c r="Q60"/>
-      <c r="R60"/>
-      <c r="S60"/>
-      <c r="T60"/>
-      <c r="U60"/>
-      <c r="V60" s="2"/>
-      <c r="W60"/>
-      <c r="X60"/>
-      <c r="Y60"/>
-      <c r="Z60"/>
-      <c r="AA60"/>
-      <c r="AB60"/>
-      <c r="AC60"/>
-      <c r="AD60"/>
-      <c r="AE60"/>
-      <c r="AF60"/>
-      <c r="AG60" s="2"/>
-      <c r="AH60"/>
-      <c r="AI60"/>
-      <c r="AJ60"/>
-      <c r="AK60"/>
-      <c r="AL60"/>
-      <c r="AM60"/>
-      <c r="AN60"/>
-      <c r="AO60"/>
-      <c r="AP60"/>
-      <c r="AQ60"/>
-      <c r="AR60" s="2"/>
-      <c r="AS60"/>
-      <c r="AT60"/>
-      <c r="AU60"/>
-      <c r="AV60"/>
-      <c r="AW60"/>
-      <c r="AX60"/>
-      <c r="AY60"/>
-      <c r="AZ60"/>
-      <c r="BA60"/>
-      <c r="BB60"/>
-      <c r="BC60" s="2"/>
-      <c r="BD60"/>
-      <c r="BE60"/>
-      <c r="BF60"/>
-      <c r="BG60"/>
-      <c r="BH60"/>
-      <c r="BI60"/>
-      <c r="BJ60"/>
-      <c r="BK60"/>
-      <c r="BL60"/>
-      <c r="BM60"/>
-      <c r="BN60" s="2"/>
-      <c r="BO60"/>
-      <c r="BP60"/>
-      <c r="BQ60"/>
-      <c r="BR60"/>
-      <c r="BS60"/>
-      <c r="BT60"/>
-      <c r="BU60"/>
-      <c r="BV60"/>
-      <c r="BW60"/>
-      <c r="BX60"/>
-      <c r="BY60" s="2"/>
-      <c r="BZ60"/>
-      <c r="CA60"/>
-      <c r="CB60"/>
-      <c r="CC60"/>
-      <c r="CD60"/>
-      <c r="CE60"/>
-      <c r="CF60"/>
-      <c r="CG60"/>
-      <c r="CH60"/>
-      <c r="CI60"/>
-      <c r="CJ60" s="2"/>
-      <c r="CK60"/>
-      <c r="CL60"/>
-      <c r="CM60"/>
-      <c r="CN60"/>
-      <c r="CO60"/>
-      <c r="CP60"/>
-      <c r="CQ60"/>
-      <c r="CR60"/>
-      <c r="CS60"/>
-      <c r="CT60"/>
-      <c r="CU60" s="2"/>
-      <c r="CV60"/>
-      <c r="CW60"/>
-      <c r="CX60"/>
-      <c r="CY60"/>
-      <c r="CZ60"/>
-      <c r="DA60"/>
-      <c r="DB60"/>
-      <c r="DC60"/>
-      <c r="DD60"/>
-      <c r="DE60"/>
-      <c r="DF60"/>
-      <c r="DG60"/>
-      <c r="DH60"/>
-      <c r="DI60"/>
-      <c r="DJ60"/>
-      <c r="DK60"/>
-      <c r="DL60"/>
-      <c r="DM60"/>
-      <c r="DN60"/>
-      <c r="DO60"/>
-      <c r="DP60"/>
-      <c r="DQ60" s="2"/>
-      <c r="DR60"/>
-      <c r="DS60"/>
-      <c r="DT60"/>
-      <c r="DU60"/>
-      <c r="DV60"/>
-      <c r="DW60"/>
-    </row>
-    <row r="61" spans="1:127" s="60" customFormat="1" x14ac:dyDescent="0.5">
-      <c r="A61" s="79"/>
-      <c r="B61" s="79"/>
-      <c r="C61" s="79"/>
-      <c r="D61" s="80"/>
-      <c r="E61"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="53"/>
-      <c r="H61"/>
-      <c r="I61"/>
-      <c r="J61"/>
-      <c r="K61" s="2"/>
-      <c r="L61"/>
-      <c r="M61"/>
-      <c r="N61"/>
-      <c r="O61"/>
-      <c r="P61"/>
-      <c r="Q61"/>
-      <c r="R61" s="53"/>
-      <c r="S61"/>
-      <c r="T61"/>
-      <c r="U61"/>
-      <c r="V61" s="2"/>
-      <c r="W61"/>
-      <c r="X61"/>
-      <c r="Y61"/>
-      <c r="Z61"/>
-      <c r="AA61"/>
-      <c r="AB61"/>
-      <c r="AC61" s="53"/>
-      <c r="AD61"/>
-      <c r="AE61"/>
-      <c r="AF61"/>
-      <c r="AG61" s="2"/>
-      <c r="AH61"/>
-      <c r="AI61"/>
-      <c r="AJ61"/>
-      <c r="AK61"/>
-      <c r="AL61"/>
-      <c r="AM61"/>
-      <c r="AN61" s="53"/>
-      <c r="AO61"/>
-      <c r="AP61"/>
-      <c r="AQ61"/>
-      <c r="AR61" s="2"/>
-      <c r="AS61"/>
-      <c r="AT61"/>
-      <c r="AU61"/>
-      <c r="AV61"/>
-      <c r="AW61"/>
-      <c r="AX61"/>
-      <c r="AY61" s="53"/>
-      <c r="AZ61"/>
-      <c r="BA61"/>
-      <c r="BB61"/>
-      <c r="BC61" s="2"/>
-      <c r="BD61"/>
-      <c r="BE61"/>
-      <c r="BF61"/>
-      <c r="BG61"/>
-      <c r="BH61"/>
-      <c r="BI61"/>
-      <c r="BJ61" s="53"/>
-      <c r="BK61"/>
-      <c r="BL61"/>
-      <c r="BM61"/>
-      <c r="BN61" s="2"/>
-      <c r="BO61"/>
-      <c r="BP61"/>
-      <c r="BQ61"/>
-      <c r="BR61"/>
-      <c r="BS61"/>
-      <c r="BT61"/>
-      <c r="BU61" s="53"/>
-      <c r="BV61"/>
-      <c r="BW61"/>
-      <c r="BX61"/>
-      <c r="BY61" s="2"/>
-      <c r="BZ61"/>
-      <c r="CA61"/>
-      <c r="CB61"/>
-      <c r="CC61"/>
-      <c r="CD61"/>
-      <c r="CE61"/>
-      <c r="CF61" s="53"/>
-      <c r="CG61"/>
-      <c r="CH61"/>
-      <c r="CI61"/>
-      <c r="CJ61" s="2"/>
-      <c r="CK61"/>
-      <c r="CL61"/>
-      <c r="CM61"/>
-      <c r="CN61"/>
-      <c r="CO61"/>
-      <c r="CP61"/>
-      <c r="CQ61" s="53"/>
-      <c r="CR61"/>
-      <c r="CS61"/>
-      <c r="CT61"/>
-      <c r="CU61" s="2"/>
-      <c r="CV61"/>
-      <c r="CW61"/>
-      <c r="CX61"/>
-      <c r="CY61"/>
-      <c r="CZ61"/>
-      <c r="DA61"/>
-      <c r="DB61" s="53"/>
-      <c r="DC61" s="53"/>
-      <c r="DD61" s="53"/>
-      <c r="DE61" s="53"/>
-      <c r="DF61" s="53"/>
-      <c r="DG61" s="53"/>
-      <c r="DH61" s="53"/>
-      <c r="DI61"/>
-      <c r="DJ61"/>
-      <c r="DK61"/>
-      <c r="DL61"/>
-      <c r="DM61" s="53"/>
-      <c r="DN61"/>
-      <c r="DO61"/>
-      <c r="DP61"/>
-      <c r="DQ61" s="2"/>
-      <c r="DR61"/>
-      <c r="DS61"/>
-      <c r="DT61"/>
-      <c r="DU61"/>
-      <c r="DV61"/>
-      <c r="DW61"/>
-    </row>
-    <row r="62" spans="1:127" x14ac:dyDescent="0.5">
-      <c r="A62" s="79"/>
-      <c r="B62" s="79"/>
-      <c r="C62" s="79"/>
-      <c r="D62" s="80"/>
-    </row>
-    <row r="63" spans="1:127" x14ac:dyDescent="0.5">
-      <c r="A63" s="79"/>
-      <c r="B63" s="79"/>
-      <c r="C63" s="79"/>
-      <c r="K63"/>
-      <c r="V63"/>
-      <c r="AG63"/>
-      <c r="AR63"/>
-      <c r="BC63"/>
-      <c r="BN63"/>
-      <c r="BY63"/>
-      <c r="CJ63"/>
-      <c r="CU63"/>
-      <c r="DF63"/>
-      <c r="DQ63"/>
+      <c r="K56"/>
+      <c r="V56"/>
+      <c r="AG56"/>
+      <c r="AR56"/>
+      <c r="BC56"/>
+      <c r="BN56"/>
+      <c r="BY56"/>
+      <c r="CJ56"/>
+      <c r="CU56"/>
+      <c r="DF56"/>
+      <c r="DQ56"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>